<commit_message>
Reports for online passing
</commit_message>
<xml_diff>
--- a/lab4/Lab4.xlsx
+++ b/lab4/Lab4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\vpo\lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4023CC20-6E79-4E9C-B28E-6C4F84291478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9201F78D-3CBE-41C5-BFA3-FE9F608477F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="114">
   <si>
     <t>Идентификатор</t>
   </si>
@@ -298,12 +298,6 @@
 Дефект: игнорирование нажатия на кнопку смены языка, при повторном нажатии</t>
   </si>
   <si>
-    <t>Калькулятор</t>
-  </si>
-  <si>
-    <t>dump</t>
-  </si>
-  <si>
     <t>1.В текстовом редакторе Windows написать строку "HGDддыфЫФв". 2. Скопировать её в Element. Дефект: недопустимые значения</t>
   </si>
   <si>
@@ -362,9 +356,6 @@
   </si>
   <si>
     <t>1. Добавить элемент abc, ac и cbaa. 2. Добавить фильтр a в "голову строки". Дефект: некорректный вывод списка элементов.</t>
-  </si>
-  <si>
-    <t>File Researcher</t>
   </si>
   <si>
     <t>Кнопка с цифрой ‘2’ выглядит отлично от других цифр</t>
@@ -941,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M80" sqref="M80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,22 +1011,20 @@
       <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="11" t="s">
-        <v>83</v>
-      </c>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>14</v>
@@ -1067,7 +1056,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>29</v>
@@ -1099,13 +1088,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>14</v>
@@ -1210,7 +1199,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>14</v>
@@ -1239,13 +1228,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>14</v>
@@ -1274,10 +1263,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>32</v>
@@ -1385,7 +1374,7 @@
         <v>41</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>14</v>
@@ -1414,13 +1403,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>14</v>
@@ -1449,13 +1438,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>14</v>
@@ -1583,9 +1572,7 @@
       <c r="K18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="10" t="s">
-        <v>82</v>
-      </c>
+      <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" ht="204" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
@@ -1627,13 +1614,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>14</v>
@@ -1767,13 +1754,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>14</v>
@@ -1802,13 +1789,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>14</v>
@@ -1866,9 +1853,7 @@
       <c r="K26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="9" t="s">
-        <v>104</v>
-      </c>
+      <c r="L26" s="9"/>
     </row>
     <row r="27" spans="1:12" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
@@ -1980,13 +1965,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>14</v>

</xml_diff>